<commit_message>
modified CAD model, deleteing the old sprocket for 1/4-20 and adding the new sprocket file for the 3/8-16. NOTE: NEED TO CHANGE THREADED ROD TO 3/8-16 ON THE CAD
</commit_message>
<xml_diff>
--- a/Documentation/Motor Specs Charts.xlsx
+++ b/Documentation/Motor Specs Charts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Dropbox\ME102b\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Documents\GitHub\blob\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>No Load Speed (RPM)</t>
   </si>
@@ -119,9 +119,6 @@
     <t>2_1</t>
   </si>
   <si>
-    <t>1_1</t>
-  </si>
-  <si>
     <t>Motor</t>
   </si>
   <si>
@@ -146,12 +143,6 @@
     <t>Stall Current (A)</t>
   </si>
   <si>
-    <t>% of max torque 2.5454</t>
-  </si>
-  <si>
-    <t>% of max torque 3.1806</t>
-  </si>
-  <si>
     <t>Drive Speed (RPM)</t>
   </si>
   <si>
@@ -166,6 +157,24 @@
   <si>
     <t>Linear speed (in/sec)</t>
   </si>
+  <si>
+    <t>F*V=(.85)*Tau*omega</t>
+  </si>
+  <si>
+    <t>RPM @ 1in/sec torque</t>
+  </si>
+  <si>
+    <t>1_1.5</t>
+  </si>
+  <si>
+    <t>% of max torque 3.781</t>
+  </si>
+  <si>
+    <t>% of max torque 5.05116</t>
+  </si>
+  <si>
+    <t>% of max torque 6.3191</t>
+  </si>
 </sst>
 </file>
 
@@ -173,7 +182,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -191,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +216,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEAAAAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,7 +304,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -297,9 +324,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -309,25 +333,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -336,10 +348,35 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -790,8 +827,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="609062352"/>
-        <c:axId val="609062896"/>
+        <c:axId val="325227832"/>
+        <c:axId val="325230184"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1786,7 +1823,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="609062352"/>
+        <c:axId val="325227832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1843,12 +1880,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609062896"/>
+        <c:crossAx val="325230184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="609062896"/>
+        <c:axId val="325230184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,7 +1942,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609062352"/>
+        <c:crossAx val="325227832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2274,8 +2311,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="440463440"/>
-        <c:axId val="440463984"/>
+        <c:axId val="325228224"/>
+        <c:axId val="325226656"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -2914,7 +2951,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="440463440"/>
+        <c:axId val="325228224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2971,12 +3008,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440463984"/>
+        <c:crossAx val="325226656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="440463984"/>
+        <c:axId val="325226656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3033,7 +3070,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440463440"/>
+        <c:crossAx val="325228224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3219,7 +3256,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.1806000000000001</c:v>
+                  <c:v>6.3190999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3231,7 +3268,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>720</c:v>
+                  <c:v>552</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3273,7 +3310,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.9075</c:v>
+                  <c:v>3.7810000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3285,7 +3322,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1200</c:v>
+                  <c:v>960</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3331,7 +3368,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5453999999999999</c:v>
+                  <c:v>5.0511600000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3343,7 +3380,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>900</c:v>
+                  <c:v>720</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3358,8 +3395,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="664439440"/>
-        <c:axId val="664444336"/>
+        <c:axId val="325229400"/>
+        <c:axId val="325230968"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -3672,7 +3709,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="664439440"/>
+        <c:axId val="325229400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3729,12 +3766,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664444336"/>
+        <c:crossAx val="325230968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="664444336"/>
+        <c:axId val="325230968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3791,7 +3828,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664439440"/>
+        <c:crossAx val="325229400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4005,7 +4042,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.1806000000000001</c:v>
+                  <c:v>6.3190999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4017,7 +4054,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>720</c:v>
+                  <c:v>552</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4059,7 +4096,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5453999999999999</c:v>
+                  <c:v>5.0511600000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4071,9 +4108,69 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>900</c:v>
+                  <c:v>720</c:v>
                 </c:pt>
               </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>1in/sec</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.7810000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>960</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
@@ -4128,8 +4225,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.7121440081871431E-2"/>
-                  <c:y val="-0.12617545596584318"/>
+                  <c:x val="0.11112630593538772"/>
+                  <c:y val="-0.1483582529711876"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4172,7 +4269,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>11.333333333333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4184,7 +4281,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -4334,87 +4431,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="664443792"/>
-        <c:axId val="664432912"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="3"/>
-                <c:order val="3"/>
-                <c:tx>
-                  <c:v>1in/sec</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="25400" cap="rnd">
-                    <a:noFill/>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent6">
-                        <a:lumMod val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent6">
-                          <a:lumMod val="60000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$40</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>1.9075</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$40</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>1200</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
+        <c:axId val="325230576"/>
+        <c:axId val="325231360"/>
+        <c:extLst/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="664443792"/>
+        <c:axId val="325230576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4546,12 +4568,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664432912"/>
+        <c:crossAx val="325231360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="664432912"/>
+        <c:axId val="325231360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4678,7 +4700,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664443792"/>
+        <c:crossAx val="325230576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4697,15 +4719,15 @@
         <c:delete val="1"/>
       </c:legendEntry>
       <c:legendEntry>
-        <c:idx val="3"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
         <c:idx val="4"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:legendEntry>
-        <c:idx val="8"/>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:layout/>
@@ -7006,7 +7028,7 @@
       <xdr:rowOff>398145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>32385</xdr:rowOff>
@@ -7036,7 +7058,7 @@
       <xdr:rowOff>116205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>3810</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>116205</xdr:rowOff>
@@ -7066,7 +7088,7 @@
       <xdr:rowOff>181841</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>69273</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -7096,7 +7118,7 @@
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
@@ -7384,30 +7406,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q59"/>
+  <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O61" sqref="O61"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S57" sqref="S57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.89453125" customWidth="1"/>
+    <col min="2" max="2" width="10.89453125" customWidth="1"/>
+    <col min="3" max="3" width="7.20703125" customWidth="1"/>
+    <col min="4" max="4" width="7.68359375" customWidth="1"/>
+    <col min="5" max="5" width="8.1015625" customWidth="1"/>
+    <col min="6" max="6" width="6.3125" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="6.88671875" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="8.20703125" customWidth="1"/>
+    <col min="9" max="9" width="8.3125" customWidth="1"/>
+    <col min="10" max="10" width="7.68359375" customWidth="1"/>
+    <col min="11" max="11" width="8.41796875" customWidth="1"/>
+    <col min="12" max="14" width="6.89453125" customWidth="1"/>
+    <col min="15" max="15" width="8.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -7424,7 +7446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -7440,8 +7462,11 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="V2" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -7458,7 +7483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -7474,12 +7499,12 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="Q4">
+      <c r="T4">
         <f>17/4</f>
         <v>4.25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -7495,12 +7520,12 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="Q5">
+      <c r="T5">
         <f>17/3</f>
         <v>5.666666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -7517,7 +7542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -7534,7 +7559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -7551,7 +7576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -7568,7 +7593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -7585,7 +7610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -7602,7 +7627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -7619,7 +7644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -7636,7 +7661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -7653,7 +7678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="B15">
         <v>3.1806000000000001</v>
       </c>
@@ -7661,7 +7686,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="B16">
         <v>1.9075</v>
       </c>
@@ -7669,7 +7694,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B17">
         <v>2.5453999999999999</v>
       </c>
@@ -7677,13 +7702,13 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -7700,7 +7725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -7717,7 +7742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -7736,7 +7761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -7753,7 +7778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -7770,7 +7795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -7787,7 +7812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -7804,7 +7829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -7821,7 +7846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B28">
         <v>3.1806000000000001</v>
       </c>
@@ -7829,7 +7854,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B29">
         <v>1.9075</v>
       </c>
@@ -7837,7 +7862,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B30">
         <v>2.5453999999999999</v>
       </c>
@@ -7845,7 +7870,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -7862,7 +7887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -7881,7 +7906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -7900,7 +7925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -7919,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>27</v>
       </c>
@@ -7938,31 +7963,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>0.6</v>
+      </c>
       <c r="B39">
-        <v>3.1806000000000001</v>
+        <v>6.3190999999999997</v>
       </c>
       <c r="C39">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>3.7810000000000001</v>
+      </c>
+      <c r="C40">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>0.75</v>
+      </c>
+      <c r="B41">
+        <v>5.0511600000000003</v>
+      </c>
+      <c r="C41">
         <v>720</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B40">
-        <v>1.9075</v>
-      </c>
-      <c r="C40">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B41">
-        <v>2.5453999999999999</v>
-      </c>
-      <c r="C41">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -7972,56 +8006,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D54" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G54" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J54" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K54" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L54" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M54" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H54" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I54" s="7" t="s">
+      <c r="N54" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="J54" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="K54" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="L54" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="M54" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="N54" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="O54" s="7" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="P54" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q54" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="R54" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B55" s="8">
         <f>84</f>
@@ -8039,7 +8082,7 @@
         <f>C55*2</f>
         <v>1000</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="F55" s="10" t="s">
         <v>30</v>
       </c>
       <c r="G55" s="8">
@@ -8048,153 +8091,193 @@
       <c r="H55" s="8">
         <v>5</v>
       </c>
-      <c r="I55" s="12">
-        <f>(-23.81*2.5454)+1000</f>
-        <v>939.39402600000005</v>
-      </c>
-      <c r="J55" s="15">
-        <f>(I55/60)/20</f>
-        <v>0.78282835500000003</v>
-      </c>
-      <c r="K55" s="12">
-        <f>(-23.81*3.1806)+1000</f>
-        <v>924.26991399999997</v>
-      </c>
-      <c r="L55" s="15">
-        <f>(K55/60)/20</f>
-        <v>0.77022492833333334</v>
-      </c>
-      <c r="M55" s="18">
-        <f>2.5454/42</f>
-        <v>6.0604761904761904E-2</v>
-      </c>
-      <c r="N55" s="18">
-        <f>3.1806/42</f>
-        <v>7.5728571428571437E-2</v>
-      </c>
-      <c r="O55" s="21">
+      <c r="I55" s="11">
+        <f>(-23.81*5.05116)+1000</f>
+        <v>879.73188040000002</v>
+      </c>
+      <c r="J55" s="13">
+        <f>(I55/60)/16</f>
+        <v>0.91638737541666671</v>
+      </c>
+      <c r="K55" s="11">
+        <f>(-23.81*6.3191)+1000</f>
+        <v>849.54222900000002</v>
+      </c>
+      <c r="L55" s="13">
+        <f>(K55/60)/16</f>
+        <v>0.88493982187499998</v>
+      </c>
+      <c r="M55" s="11">
+        <f>(-23.81*3.781)+1000</f>
+        <v>909.97438999999997</v>
+      </c>
+      <c r="N55" s="13">
+        <f>(M55/60)/16</f>
+        <v>0.94788998958333326</v>
+      </c>
+      <c r="O55" s="14">
+        <f>5.05116/D55</f>
+        <v>0.1202657142857143</v>
+      </c>
+      <c r="P55" s="14">
+        <f>6.3191/D55</f>
+        <v>0.1504547619047619</v>
+      </c>
+      <c r="Q55" s="24">
+        <f>3.781/D55</f>
+        <v>9.0023809523809534E-2</v>
+      </c>
+      <c r="R55" s="16">
         <v>39.950000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A56" s="9" t="s">
+    <row r="56" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" s="19">
+        <v>17</v>
+      </c>
+      <c r="C56" s="19">
+        <v>1000</v>
+      </c>
+      <c r="D56" s="19">
+        <f>B56/1.5</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="E56" s="19">
+        <f>C56*1.5</f>
+        <v>1500</v>
+      </c>
+      <c r="F56" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G56" s="19">
+        <v>6</v>
+      </c>
+      <c r="H56" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="I56" s="20">
+        <f>(-132.35*5.05116)+1500</f>
+        <v>831.47897399999999</v>
+      </c>
+      <c r="J56" s="21">
+        <f t="shared" ref="J56:J57" si="0">(I56/60)/16</f>
+        <v>0.86612393124999998</v>
+      </c>
+      <c r="K56" s="20">
+        <f>(-132.35*6.3191)+1500</f>
+        <v>663.66711500000008</v>
+      </c>
+      <c r="L56" s="21">
+        <f t="shared" ref="L56:L57" si="1">(K56/60)/16</f>
+        <v>0.69131991145833338</v>
+      </c>
+      <c r="M56" s="20">
+        <f>(-132.35*3.781)+1500</f>
+        <v>999.58465000000001</v>
+      </c>
+      <c r="N56" s="21">
+        <f t="shared" ref="N56:N57" si="2">(M56/60)/16</f>
+        <v>1.0412340104166666</v>
+      </c>
+      <c r="O56" s="26">
+        <f>5.05116/D56</f>
+        <v>0.44569058823529412</v>
+      </c>
+      <c r="P56" s="25">
+        <f t="shared" ref="P56:P57" si="3">6.3191/D56</f>
+        <v>0.55756764705882345</v>
+      </c>
+      <c r="Q56" s="27">
+        <f>3.781/D56</f>
+        <v>0.33361764705882352</v>
+      </c>
+      <c r="R56" s="22">
+        <v>36.950000000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B56" s="9">
-        <v>17</v>
-      </c>
-      <c r="C56" s="9">
-        <v>1000</v>
-      </c>
-      <c r="D56" s="9">
-        <f>B56/1</f>
-        <v>17</v>
-      </c>
-      <c r="E56" s="9">
-        <f>C56*1</f>
-        <v>1000</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G56" s="9">
-        <v>6</v>
-      </c>
-      <c r="H56" s="9">
-        <v>6.5</v>
-      </c>
-      <c r="I56" s="13">
-        <f>(-58.824*2.5454)+1000</f>
-        <v>850.26939040000002</v>
-      </c>
-      <c r="J56" s="16">
-        <f t="shared" ref="J56:J57" si="0">(I56/60)/20</f>
-        <v>0.70855782533333334</v>
-      </c>
-      <c r="K56" s="13">
-        <f>(-58.824*3.1806)+1000</f>
-        <v>812.90438560000007</v>
-      </c>
-      <c r="L56" s="16">
-        <f t="shared" ref="L56:L57" si="1">(K56/60)/20</f>
-        <v>0.67742032133333341</v>
-      </c>
-      <c r="M56" s="19">
-        <f>2.5454/17</f>
-        <v>0.14972941176470589</v>
-      </c>
-      <c r="N56" s="19">
-        <f>3.1806/17</f>
-        <v>0.18709411764705883</v>
-      </c>
-      <c r="O56" s="22">
-        <v>36.950000000000003</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B57" s="10">
+      <c r="B57" s="9">
         <v>11</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="9">
         <v>630</v>
       </c>
-      <c r="D57" s="10">
+      <c r="D57" s="9">
         <f>B57/2</f>
         <v>5.5</v>
       </c>
-      <c r="E57" s="10">
+      <c r="E57" s="9">
         <f>C57*2</f>
         <v>1260</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G57" s="10">
+      <c r="G57" s="9">
         <v>6</v>
       </c>
-      <c r="H57" s="10">
+      <c r="H57" s="9">
         <v>2.4</v>
       </c>
-      <c r="I57" s="14">
-        <f>(-229.09*2.5454)+1260</f>
-        <v>676.87431400000003</v>
-      </c>
-      <c r="J57" s="17">
+      <c r="I57" s="12">
+        <f>(-229.09*5.05116)+1260</f>
+        <v>102.8297556</v>
+      </c>
+      <c r="J57" s="13">
         <f t="shared" si="0"/>
-        <v>0.56406192833333335</v>
-      </c>
-      <c r="K57" s="14">
-        <f>(-229.09*3.1806)+1260</f>
-        <v>531.35634599999992</v>
-      </c>
-      <c r="L57" s="17">
+        <v>0.10711432875</v>
+      </c>
+      <c r="K57" s="12">
+        <f>(-229.09*6.3191)+1260</f>
+        <v>-187.64261899999997</v>
+      </c>
+      <c r="L57" s="13">
         <f t="shared" si="1"/>
-        <v>0.44279695499999994</v>
-      </c>
-      <c r="M57" s="20">
-        <f>2.5454/5.5</f>
-        <v>0.46279999999999999</v>
-      </c>
-      <c r="N57" s="20">
-        <f>3.1806/5.5</f>
-        <v>0.57829090909090908</v>
-      </c>
-      <c r="O57" s="23">
+        <v>-0.19546106145833331</v>
+      </c>
+      <c r="M57" s="12">
+        <f>(-229.09*3.781)+1260</f>
+        <v>393.81070999999997</v>
+      </c>
+      <c r="N57" s="13">
+        <f t="shared" si="2"/>
+        <v>0.41021948958333332</v>
+      </c>
+      <c r="O57" s="15">
+        <f>5.05116/D57</f>
+        <v>0.91839272727272736</v>
+      </c>
+      <c r="P57" s="25">
+        <f t="shared" si="3"/>
+        <v>1.1489272727272726</v>
+      </c>
+      <c r="Q57" s="18">
+        <f>3.781/D57</f>
+        <v>0.68745454545454543</v>
+      </c>
+      <c r="R57" s="17">
         <v>34.950000000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
+      <c r="T58">
+        <f>1200/(60*16)</f>
+        <v>1.25</v>
+      </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -8202,12 +8285,15 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="T62">
+        <f>2.5454/28</f>
+        <v>9.0907142857142853E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="K55:K57 D56:E56" formula="1"/>
-  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the Major CADs as well as did some work in properly defining some features. Aded fasteners and sprockets, made modifications as saw fit.
</commit_message>
<xml_diff>
--- a/Documentation/Motor Specs Charts.xlsx
+++ b/Documentation/Motor Specs Charts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Documents\GitHub\blob\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\blob\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -164,9 +164,6 @@
     <t>RPM @ 1in/sec torque</t>
   </si>
   <si>
-    <t>1_1.5</t>
-  </si>
-  <si>
     <t>% of max torque 3.781</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>% of max torque 6.3191</t>
+  </si>
+  <si>
+    <t>1.5_1</t>
   </si>
 </sst>
 </file>
@@ -304,7 +304,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -379,6 +379,9 @@
     <xf numFmtId="9" fontId="0" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -425,17 +428,18 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>Sheet1!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9.7=1 HP</c:v>
+                  <c:v>4.4=1 HP</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -450,11 +454,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -464,7 +468,7 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -478,126 +482,7 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>(Sheet1!$B$4,Sheet1!$D$4)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>(Sheet1!$C$4,Sheet1!$E$4)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>9.7=1 LP</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -609,7 +494,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>(Sheet1!$B$10,Sheet1!$D$10)</c:f>
+              <c:f>(Sheet1!$B$3,Sheet1!$D$3)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -617,24 +502,26 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$C$10,Sheet1!$E$10)</c:f>
+              <c:f>(Sheet1!$C$3,Sheet1!$E$3)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>630</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
@@ -680,7 +567,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.1806000000000001</c:v>
+                  <c:v>6.3190999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -692,7 +579,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>720</c:v>
+                  <c:v>552</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -740,7 +627,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.9075</c:v>
+                  <c:v>3.7810000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -752,7 +639,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1200</c:v>
+                  <c:v>960</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -800,7 +687,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5453999999999999</c:v>
+                  <c:v>5.0511600000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -812,7 +699,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>900</c:v>
+                  <c:v>720</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -827,8 +714,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="325227832"/>
-        <c:axId val="325230184"/>
+        <c:axId val="1900135904"/>
+        <c:axId val="1900142432"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -935,21 +822,21 @@
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
+                <c:idx val="2"/>
+                <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$3</c15:sqref>
+                          <c15:sqref>Sheet1!$A$4</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>4.4=1 HP</c:v>
+                        <c:v>9.7=1 HP</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -966,11 +853,11 @@
                   <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent3"/>
                     </a:solidFill>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent2"/>
+                        <a:schemeClr val="accent3"/>
                       </a:solidFill>
                     </a:ln>
                     <a:effectLst/>
@@ -980,7 +867,7 @@
                   <c:spPr>
                     <a:ln w="19050" cap="rnd">
                       <a:solidFill>
-                        <a:schemeClr val="accent2"/>
+                        <a:schemeClr val="accent3"/>
                       </a:solidFill>
                       <a:prstDash val="sysDot"/>
                     </a:ln>
@@ -994,7 +881,7 @@
                   <c:spPr>
                     <a:ln w="19050" cap="rnd">
                       <a:solidFill>
-                        <a:schemeClr val="accent2"/>
+                        <a:schemeClr val="accent3"/>
                       </a:solidFill>
                       <a:prstDash val="sysDot"/>
                     </a:ln>
@@ -1002,14 +889,45 @@
                   </c:spPr>
                   <c:trendlineType val="linear"/>
                   <c:dispRSqr val="0"/>
-                  <c:dispEq val="0"/>
+                  <c:dispEq val="1"/>
+                  <c:trendlineLbl>
+                    <c:layout/>
+                    <c:numFmt formatCode="General" sourceLinked="0"/>
+                    <c:spPr>
+                      <a:noFill/>
+                      <a:ln>
+                        <a:noFill/>
+                      </a:ln>
+                      <a:effectLst/>
+                    </c:spPr>
+                    <c:txPr>
+                      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                      <a:lstStyle/>
+                      <a:p>
+                        <a:pPr>
+                          <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="65000"/>
+                                <a:lumOff val="35000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:defRPr>
+                        </a:pPr>
+                        <a:endParaRPr lang="en-US"/>
+                      </a:p>
+                    </c:txPr>
+                  </c:trendlineLbl>
                 </c:trendline>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$B$3,Sheet1!$D$3)</c15:sqref>
+                          <c15:sqref>(Sheet1!$B$4,Sheet1!$D$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1020,17 +938,17 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>8</c:v>
+                        <c:v>17</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$C$3,Sheet1!$E$3)</c15:sqref>
+                          <c15:sqref>(Sheet1!$C$4,Sheet1!$E$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1038,7 +956,7 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="2"/>
                       <c:pt idx="0">
-                        <c:v>2200</c:v>
+                        <c:v>1000</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>0</c:v>
@@ -1437,6 +1355,114 @@
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
               <c15:ser>
+                <c:idx val="7"/>
+                <c:order val="7"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>9.7=1 LP</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:trendline>
+                  <c:spPr>
+                    <a:ln w="19050" cap="rnd">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:prstDash val="sysDot"/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:trendlineType val="linear"/>
+                  <c:dispRSqr val="0"/>
+                  <c:dispEq val="0"/>
+                </c:trendline>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(Sheet1!$B$10,Sheet1!$D$10)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>11</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>(Sheet1!$C$10,Sheet1!$E$10)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>630</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
                 <c:idx val="8"/>
                 <c:order val="8"/>
                 <c:tx>
@@ -1823,7 +1849,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="325227832"/>
+        <c:axId val="1900135904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1880,12 +1906,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325230184"/>
+        <c:crossAx val="1900142432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="325230184"/>
+        <c:axId val="1900142432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1942,7 +1968,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325227832"/>
+        <c:crossAx val="1900135904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1954,6 +1980,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2168,7 +2226,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.1806000000000001</c:v>
+                  <c:v>6.3190999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2180,7 +2238,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>720</c:v>
+                  <c:v>552</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2226,7 +2284,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.9075</c:v>
+                  <c:v>3.7810000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2238,7 +2296,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1200</c:v>
+                  <c:v>960</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2284,7 +2342,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5453999999999999</c:v>
+                  <c:v>5.0511600000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2296,7 +2354,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>900</c:v>
+                  <c:v>720</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2311,8 +2369,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="325228224"/>
-        <c:axId val="325226656"/>
+        <c:axId val="1900141344"/>
+        <c:axId val="1900137536"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -2951,7 +3009,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="325228224"/>
+        <c:axId val="1900141344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3008,12 +3066,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325226656"/>
+        <c:crossAx val="1900137536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="325226656"/>
+        <c:axId val="1900137536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3070,7 +3128,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325228224"/>
+        <c:crossAx val="1900141344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3395,8 +3453,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="325229400"/>
-        <c:axId val="325230968"/>
+        <c:axId val="1900146784"/>
+        <c:axId val="1900145152"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -3709,7 +3767,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="325229400"/>
+        <c:axId val="1900146784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3766,12 +3824,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325230968"/>
+        <c:crossAx val="1900145152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="325230968"/>
+        <c:axId val="1900145152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3828,7 +3886,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325229400"/>
+        <c:crossAx val="1900146784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4401,7 +4459,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4413,7 +4471,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1260</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -4431,12 +4489,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="325230576"/>
-        <c:axId val="325231360"/>
+        <c:axId val="1900144064"/>
+        <c:axId val="1900140800"/>
         <c:extLst/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="325230576"/>
+        <c:axId val="1900144064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4568,12 +4626,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325231360"/>
+        <c:crossAx val="1900140800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="325231360"/>
+        <c:axId val="1900140800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4700,7 +4758,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325230576"/>
+        <c:crossAx val="1900144064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7408,28 +7466,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S57" sqref="S57"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.89453125" customWidth="1"/>
-    <col min="2" max="2" width="10.89453125" customWidth="1"/>
-    <col min="3" max="3" width="7.20703125" customWidth="1"/>
-    <col min="4" max="4" width="7.68359375" customWidth="1"/>
-    <col min="5" max="5" width="8.1015625" customWidth="1"/>
-    <col min="6" max="6" width="6.3125" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="8.20703125" customWidth="1"/>
-    <col min="9" max="9" width="8.3125" customWidth="1"/>
-    <col min="10" max="10" width="7.68359375" customWidth="1"/>
-    <col min="11" max="11" width="8.41796875" customWidth="1"/>
-    <col min="12" max="14" width="6.89453125" customWidth="1"/>
-    <col min="15" max="15" width="8.89453125" customWidth="1"/>
+    <col min="8" max="8" width="8.21875" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" customWidth="1"/>
+    <col min="12" max="14" width="6.88671875" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -7446,7 +7504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -7466,7 +7524,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -7483,7 +7541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -7504,7 +7562,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -7525,7 +7583,7 @@
         <v>5.666666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -7542,7 +7600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -7559,7 +7617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -7576,7 +7634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -7593,7 +7651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -7610,7 +7668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -7627,7 +7685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -7644,7 +7702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -7661,7 +7719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -7678,37 +7736,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.6</v>
+      </c>
       <c r="B15">
-        <v>3.1806000000000001</v>
+        <v>6.3190999999999997</v>
       </c>
       <c r="C15">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>3.7810000000000001</v>
+      </c>
+      <c r="C16">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0.75</v>
+      </c>
+      <c r="B17">
+        <v>5.0511600000000003</v>
+      </c>
+      <c r="C17">
         <v>720</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16">
-        <v>1.9075</v>
-      </c>
-      <c r="C16">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17">
-        <v>2.5453999999999999</v>
-      </c>
-      <c r="C17">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -7725,7 +7792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -7742,7 +7809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -7761,7 +7828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -7778,7 +7845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -7795,7 +7862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -7812,7 +7879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -7829,7 +7896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -7846,31 +7913,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0.6</v>
+      </c>
       <c r="B28">
-        <v>3.1806000000000001</v>
+        <v>6.3190999999999997</v>
       </c>
       <c r="C28">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>3.7810000000000001</v>
+      </c>
+      <c r="C29">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0.75</v>
+      </c>
+      <c r="B30">
+        <v>5.0511600000000003</v>
+      </c>
+      <c r="C30">
         <v>720</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29">
-        <v>1.9075</v>
-      </c>
-      <c r="C29">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30">
-        <v>2.5453999999999999</v>
-      </c>
-      <c r="C30">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -7887,7 +7963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -7906,7 +7982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -7925,7 +8001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -7944,7 +8020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>27</v>
       </c>
@@ -7963,7 +8039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0.6</v>
       </c>
@@ -7974,7 +8050,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1</v>
       </c>
@@ -7985,7 +8061,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0.75</v>
       </c>
@@ -7996,7 +8072,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -8006,7 +8082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>31</v>
       </c>
@@ -8050,19 +8126,19 @@
         <v>43</v>
       </c>
       <c r="O54" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="P54" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="P54" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="Q54" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R54" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>32</v>
       </c>
@@ -8131,7 +8207,7 @@
         <v>39.950000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="19" t="s">
         <v>33</v>
       </c>
@@ -8150,7 +8226,7 @@
         <v>1500</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G56" s="19">
         <v>6</v>
@@ -8198,7 +8274,7 @@
         <v>36.950000000000003</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
         <v>34</v>
       </c>
@@ -8209,12 +8285,12 @@
         <v>630</v>
       </c>
       <c r="D57" s="9">
-        <f>B57/2</f>
-        <v>5.5</v>
+        <f>B57</f>
+        <v>11</v>
       </c>
       <c r="E57" s="9">
-        <f>C57*2</f>
-        <v>1260</v>
+        <f>C57</f>
+        <v>630</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>30</v>
@@ -8229,7 +8305,7 @@
         <f>(-229.09*5.05116)+1260</f>
         <v>102.8297556</v>
       </c>
-      <c r="J57" s="13">
+      <c r="J57" s="28">
         <f t="shared" si="0"/>
         <v>0.10711432875</v>
       </c>
@@ -8251,21 +8327,21 @@
       </c>
       <c r="O57" s="15">
         <f>5.05116/D57</f>
-        <v>0.91839272727272736</v>
+        <v>0.45919636363636368</v>
       </c>
       <c r="P57" s="25">
         <f t="shared" si="3"/>
-        <v>1.1489272727272726</v>
+        <v>0.57446363636363629</v>
       </c>
       <c r="Q57" s="18">
         <f>3.781/D57</f>
-        <v>0.68745454545454543</v>
+        <v>0.34372727272727271</v>
       </c>
       <c r="R57" s="17">
         <v>34.950000000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -8277,7 +8353,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -8285,7 +8361,7 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="T62">
         <f>2.5454/28</f>
         <v>9.0907142857142853E-2</v>

</xml_diff>